<commit_message>
finalizing local_part... adding more tests, adding dns functions
</commit_message>
<xml_diff>
--- a/specs/email_spec.xlsx
+++ b/specs/email_spec.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12285" windowHeight="9960"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12285" windowHeight="9960" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="50">
   <si>
     <t>local-part "@" domain</t>
   </si>
@@ -903,6 +904,44 @@
         <family val="3"/>
       </rPr>
       <t xml:space="preserve"> = Let-dig [Ldh-str]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>domain</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = domain-addr / address-literal / dot-atom / domain-literal / obs-domain</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>address-spec</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = local-part "@" domain</t>
     </r>
   </si>
 </sst>
@@ -1238,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:K160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,4 +1883,135 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:H56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="2"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>